<commit_message>
alterando tabela pra fazer o pdf
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -181,8 +181,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -224,7 +224,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>254880</xdr:colOff>
+      <xdr:colOff>16200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>684000</xdr:rowOff>
     </xdr:to>
@@ -255,15 +255,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>168480</xdr:colOff>
+      <xdr:colOff>850680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>753480</xdr:colOff>
+      <xdr:colOff>1197000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>723600</xdr:rowOff>
+      <xdr:rowOff>742680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -276,7 +276,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3419640" y="0"/>
+          <a:off x="4818240" y="19080"/>
           <a:ext cx="3023280" cy="723600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -405,11 +405,15 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.8"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -531,16 +535,16 @@
     </row>
     <row r="10" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="4"/>
@@ -551,373 +555,373 @@
       <c r="A11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="16.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>

</xml_diff>

<commit_message>
criando tela para gerar folhas de ponto
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -85,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,36 +152,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -207,9 +216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>594000</xdr:colOff>
+      <xdr:colOff>593640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>684000</xdr:rowOff>
+      <xdr:rowOff>683640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -223,7 +232,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1870200" cy="684000"/>
+          <a:ext cx="1869840" cy="683640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -352,471 +361,471 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="12.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="15.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="44">

</xml_diff>

<commit_message>
alterando a tabela para ficar sem cabeçalho nem rodapé
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name=" " sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -289,9 +289,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>593280</xdr:colOff>
+      <xdr:colOff>592560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>683280</xdr:rowOff>
+      <xdr:rowOff>682560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -305,7 +305,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1869480" cy="683280"/>
+          <a:ext cx="1868760" cy="682560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -433,7 +433,7 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -937,11 +937,11 @@
     <mergeCell ref="A41:G41"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="0.7875" header="0.7875" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
preenchendo a tabela com data e dia do mes inteiro
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -288,9 +288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>594720</xdr:colOff>
+      <xdr:colOff>417960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>682200</xdr:rowOff>
+      <xdr:rowOff>681840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -304,7 +304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1868400" cy="682200"/>
+          <a:ext cx="1868040" cy="681840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -432,16 +432,16 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.48"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
preenchendo datas com horario corretamente
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -173,6 +173,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,10 +191,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -433,129 +433,129 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -564,10 +564,10 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -576,10 +576,10 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -588,10 +588,10 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -600,10 +600,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -612,10 +612,10 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -624,10 +624,10 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -636,10 +636,10 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -648,10 +648,10 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -660,10 +660,10 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -672,10 +672,10 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -684,10 +684,10 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -696,10 +696,10 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -708,10 +708,10 @@
       <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -720,10 +720,10 @@
       <c r="H21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -732,10 +732,10 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="n">
+      <c r="A23" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -744,10 +744,10 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -756,10 +756,10 @@
       <c r="H24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="n">
+      <c r="A25" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -768,10 +768,10 @@
       <c r="H25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -780,10 +780,10 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="n">
+      <c r="A27" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -792,10 +792,10 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="n">
+      <c r="A28" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -804,10 +804,10 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+      <c r="A29" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -816,10 +816,10 @@
       <c r="H29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
+      <c r="A30" s="6" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -828,10 +828,10 @@
       <c r="H30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="6" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -840,10 +840,10 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="n">
+      <c r="A32" s="6" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -852,10 +852,10 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="n">
+      <c r="A33" s="6" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -864,10 +864,10 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="n">
+      <c r="A34" s="6" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -876,10 +876,10 @@
       <c r="H34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="n">
+      <c r="A35" s="6" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -888,10 +888,10 @@
       <c r="H35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="n">
+      <c r="A36" s="6" t="n">
         <v>29</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -900,10 +900,10 @@
       <c r="H36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -912,10 +912,10 @@
       <c r="H37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="A38" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>

</xml_diff>

<commit_message>
escrevendo a tabela com cabeçalho
</commit_message>
<xml_diff>
--- a/Tabela ponto.xlsx
+++ b/Tabela ponto.xlsx
@@ -288,9 +288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>417960</xdr:colOff>
+      <xdr:colOff>417600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>681840</xdr:rowOff>
+      <xdr:rowOff>681480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -304,7 +304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1868040" cy="681840"/>
+          <a:ext cx="1867680" cy="681480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -432,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>